<commit_message>
Régression multilinéaire avec PIB et IPC
base : pondération avec CJO_5J
R : régression multilinéaire plus complexe et relecture de l'ensemble du
code de Loic
</commit_message>
<xml_diff>
--- a/R ASP/Tableau de Bord.xlsx
+++ b/R ASP/Tableau de Bord.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Loïc\Documents\GitHub\R-ASP\R ASP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Documents\GitHub\R-ASP\R ASP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24528" windowHeight="4788"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24525" windowHeight="4785"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Différents modèles</t>
   </si>
@@ -44,21 +44,6 @@
     <t>Désaisonnalisation</t>
   </si>
   <si>
-    <t>Indices de l'Insee à ajouter</t>
-  </si>
-  <si>
-    <t>Indice à la consommation Prix des voitures neuves</t>
-  </si>
-  <si>
-    <t>Indice à la consommation Prix des voitures occasion</t>
-  </si>
-  <si>
-    <t>http://www.insee.fr/fr/bases-de-donnees/bsweb/serie.asp?idbank=000637892</t>
-  </si>
-  <si>
-    <t>http://www.insee.fr/fr/bases-de-donnees/bsweb/serie.asp?idbank=000637893</t>
-  </si>
-  <si>
     <t>Simplexes</t>
   </si>
   <si>
@@ -96,6 +81,9 @@
   </si>
   <si>
     <t>à approfondir après</t>
+  </si>
+  <si>
+    <t>Etudier en détail le modèle le plus adapté, Imtot et IN n'ont pas de tendance linéaire</t>
   </si>
 </sst>
 </file>
@@ -195,6 +183,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -202,10 +194,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -226,7 +214,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -488,127 +476,111 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:H23"/>
+  <dimension ref="B3:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="42.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="78" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="5"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="6"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="7"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="3"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D8" t="s">
+      <c r="E10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E14" t="s">
+      <c r="D16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D22" t="s">
-        <v>6</v>
-      </c>
-      <c r="E22" t="s">
-        <v>7</v>
-      </c>
-      <c r="F22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="E23" t="s">
-        <v>8</v>
-      </c>
-      <c r="F23" t="s">
-        <v>10</v>
+      <c r="E21" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>